<commit_message>
any propagation direction and show rising map
</commit_message>
<xml_diff>
--- a/cfg/parameters1.xlsx
+++ b/cfg/parameters1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Dropbox\repo\aqua\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83EEC84-38F9-4B70-B092-5F69C78DB5D3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29286E59-9AF1-45F7-A642-E399DE1624CF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="0" windowWidth="14115" windowHeight="8400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3823" yWindow="0" windowWidth="14117" windowHeight="8400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -154,10 +154,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>est</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GTW smoothness term</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -251,23 +247,35 @@
   </si>
   <si>
     <t>The order of the model to correct trend in the curve</t>
+  </si>
+  <si>
+    <t>northx</t>
+  </si>
+  <si>
+    <t>northy</t>
+  </si>
+  <si>
+    <t>X cooridante for north vector</t>
+  </si>
+  <si>
+    <t>Y cooridante for north vector</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -576,13 +584,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.28515625" customWidth="1"/>
@@ -591,7 +599,7 @@
     <col min="7" max="7" width="105.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,19 +610,19 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -637,7 +645,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -660,7 +668,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -683,12 +691,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -703,15 +711,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -726,12 +734,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -746,15 +754,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -766,15 +774,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -786,9 +794,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -806,15 +814,15 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -826,10 +834,10 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -852,7 +860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -875,12 +883,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
@@ -895,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -918,12 +926,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -938,9 +946,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -961,15 +969,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19">
         <v>0.2</v>
@@ -981,15 +989,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
         <v>67</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>68</v>
-      </c>
-      <c r="C20" t="s">
-        <v>69</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1001,10 +1009,10 @@
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1012,7 +1020,7 @@
         <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1027,7 +1035,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1050,7 +1058,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1073,7 +1081,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -1081,7 +1089,7 @@
         <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="D25">
         <v>0.02</v>
@@ -1094,6 +1102,46 @@
       </c>
       <c r="G25" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>